<commit_message>
feat: add function export vue project report
</commit_message>
<xml_diff>
--- a/CEMS-Server/expenses.xlsx
+++ b/CEMS-Server/expenses.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>ลำดับ</t>
   </si>
@@ -92,21 +92,57 @@
     <t>789456</t>
   </si>
   <si>
+    <t>อยากกินลาบ</t>
+  </si>
+  <si>
+    <t>06/01/2568</t>
+  </si>
+  <si>
     <t>เบิกค่านวดขา</t>
   </si>
   <si>
     <t>bbbbbbbbbbbbbbbbbbbbbbbbbbbbb</t>
   </si>
   <si>
+    <t>ต้มอึ้งให้กินแหน่ว่ะ</t>
+  </si>
+  <si>
     <t>เบิกค่านวดคอ</t>
   </si>
   <si>
     <t>wdwdwdw</t>
   </si>
   <si>
+    <t>Pornchai Phoempoonkit</t>
+  </si>
+  <si>
+    <t>tesgtrwdkqaipfj</t>
+  </si>
+  <si>
+    <t>02/02/2546</t>
+  </si>
+  <si>
+    <t>ฟหกฟหก</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>กดเกดเ</t>
+  </si>
+  <si>
     <t>cccccccccccc</t>
   </si>
   <si>
+    <t>หกหด</t>
+  </si>
+  <si>
+    <t>CN-test01</t>
+  </si>
+  <si>
+    <t>CN-test</t>
+  </si>
+  <si>
     <t>ค่าอาหาร</t>
   </si>
   <si>
@@ -146,10 +182,10 @@
     <t>21/11/2567</t>
   </si>
   <si>
-    <t>Pornchai Phoempoonkit</t>
-  </si>
-  <si>
     <t>20/11/2567</t>
+  </si>
+  <si>
+    <t>CN-TestExample</t>
   </si>
   <si>
     <t>test approver requisition</t>
@@ -246,7 +282,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName=""/>
-  <dimension ref="A1:G93"/>
+  <dimension ref="A1:G110"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -258,7 +294,7 @@
     <col min="4" max="4" width="14.212424278259277" customWidth="1"/>
     <col min="5" max="5" width="16.035526275634766" customWidth="1"/>
     <col min="6" max="6" width="11.115262985229492" customWidth="1"/>
-    <col min="7" max="7" width="15.438056945800781" customWidth="1"/>
+    <col min="7" max="7" width="15.981985092163086" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -637,7 +673,7 @@
         <v>17</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>9</v>
@@ -646,10 +682,10 @@
         <v>15</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="G17" s="6">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="18">
@@ -660,7 +696,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>9</v>
@@ -669,10 +705,10 @@
         <v>15</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="G18" s="6">
-        <v>120</v>
+        <v>300</v>
       </c>
     </row>
     <row r="19">
@@ -683,7 +719,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>9</v>
@@ -692,10 +728,10 @@
         <v>15</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G19" s="6">
-        <v>100</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20">
@@ -715,10 +751,10 @@
         <v>15</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G20" s="6">
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21">
@@ -729,7 +765,7 @@
         <v>17</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>9</v>
@@ -741,7 +777,7 @@
         <v>21</v>
       </c>
       <c r="G21" s="6">
-        <v>100</v>
+        <v>200</v>
       </c>
     </row>
     <row r="22">
@@ -749,7 +785,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>22</v>
@@ -761,10 +797,10 @@
         <v>15</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="G22" s="6">
-        <v>20</v>
+        <v>200</v>
       </c>
     </row>
     <row r="23">
@@ -772,10 +808,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>9</v>
@@ -784,10 +820,10 @@
         <v>15</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="G23" s="6">
-        <v>1000</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24">
@@ -795,10 +831,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>9</v>
@@ -807,10 +843,10 @@
         <v>15</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="G24" s="6">
-        <v>800</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25">
@@ -818,10 +854,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>9</v>
@@ -830,10 +866,10 @@
         <v>15</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G25" s="6">
-        <v>100</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="26">
@@ -844,7 +880,7 @@
         <v>17</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>9</v>
@@ -853,10 +889,10 @@
         <v>15</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="G26" s="6">
-        <v>100</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="27">
@@ -867,7 +903,7 @@
         <v>17</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>9</v>
@@ -879,7 +915,7 @@
         <v>21</v>
       </c>
       <c r="G27" s="6">
-        <v>144</v>
+        <v>800</v>
       </c>
     </row>
     <row r="28">
@@ -890,7 +926,7 @@
         <v>17</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>9</v>
@@ -899,10 +935,10 @@
         <v>15</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="G28" s="6">
-        <v>144</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29">
@@ -913,7 +949,7 @@
         <v>17</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>9</v>
@@ -925,7 +961,7 @@
         <v>21</v>
       </c>
       <c r="G29" s="6">
-        <v>144</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30">
@@ -933,10 +969,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>9</v>
@@ -948,7 +984,7 @@
         <v>21</v>
       </c>
       <c r="G30" s="6">
-        <v>789</v>
+        <v>99999</v>
       </c>
     </row>
     <row r="31">
@@ -956,7 +992,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>20</v>
@@ -971,7 +1007,7 @@
         <v>21</v>
       </c>
       <c r="G31" s="6">
-        <v>12</v>
+        <v>144</v>
       </c>
     </row>
     <row r="32">
@@ -1005,7 +1041,7 @@
         <v>17</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>9</v>
@@ -1017,7 +1053,7 @@
         <v>21</v>
       </c>
       <c r="G33" s="6">
-        <v>800</v>
+        <v>144</v>
       </c>
     </row>
     <row r="34">
@@ -1028,7 +1064,7 @@
         <v>17</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>9</v>
@@ -1037,10 +1073,10 @@
         <v>15</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="G34" s="6">
-        <v>122</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35">
@@ -1051,7 +1087,7 @@
         <v>17</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>9</v>
@@ -1063,7 +1099,7 @@
         <v>21</v>
       </c>
       <c r="G35" s="6">
-        <v>200</v>
+        <v>789</v>
       </c>
     </row>
     <row r="36">
@@ -1071,7 +1107,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>20</v>
@@ -1086,7 +1122,7 @@
         <v>21</v>
       </c>
       <c r="G36" s="6">
-        <v>300</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37">
@@ -1097,7 +1133,7 @@
         <v>17</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>9</v>
@@ -1106,10 +1142,10 @@
         <v>15</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="G37" s="6">
-        <v>999</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="38">
@@ -1117,10 +1153,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>9</v>
@@ -1129,10 +1165,10 @@
         <v>15</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G38" s="6">
-        <v>114</v>
+        <v>300</v>
       </c>
     </row>
     <row r="39">
@@ -1143,7 +1179,7 @@
         <v>17</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>9</v>
@@ -1155,7 +1191,7 @@
         <v>21</v>
       </c>
       <c r="G39" s="6">
-        <v>222</v>
+        <v>144</v>
       </c>
     </row>
     <row r="40">
@@ -1166,7 +1202,7 @@
         <v>17</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>9</v>
@@ -1178,7 +1214,7 @@
         <v>21</v>
       </c>
       <c r="G40" s="6">
-        <v>123</v>
+        <v>800</v>
       </c>
     </row>
     <row r="41">
@@ -1189,7 +1225,7 @@
         <v>17</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>9</v>
@@ -1201,7 +1237,7 @@
         <v>21</v>
       </c>
       <c r="G41" s="6">
-        <v>1222</v>
+        <v>122</v>
       </c>
     </row>
     <row r="42">
@@ -1212,7 +1248,7 @@
         <v>17</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>9</v>
@@ -1224,7 +1260,7 @@
         <v>21</v>
       </c>
       <c r="G42" s="6">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="43">
@@ -1235,7 +1271,7 @@
         <v>17</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>9</v>
@@ -1244,10 +1280,10 @@
         <v>15</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="G43" s="6">
-        <v>200</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="44">
@@ -1258,7 +1294,7 @@
         <v>17</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>9</v>
@@ -1270,7 +1306,7 @@
         <v>21</v>
       </c>
       <c r="G44" s="6">
-        <v>800</v>
+        <v>300</v>
       </c>
     </row>
     <row r="45">
@@ -1293,7 +1329,7 @@
         <v>21</v>
       </c>
       <c r="G45" s="6">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="46">
@@ -1304,7 +1340,7 @@
         <v>17</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>9</v>
@@ -1313,10 +1349,10 @@
         <v>15</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G46" s="6">
-        <v>200</v>
+        <v>114</v>
       </c>
     </row>
     <row r="47">
@@ -1327,7 +1363,7 @@
         <v>17</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>9</v>
@@ -1336,10 +1372,10 @@
         <v>15</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="G47" s="6">
-        <v>122</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="48">
@@ -1362,7 +1398,7 @@
         <v>21</v>
       </c>
       <c r="G48" s="6">
-        <v>1000</v>
+        <v>222</v>
       </c>
     </row>
     <row r="49">
@@ -1373,7 +1409,7 @@
         <v>17</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>9</v>
@@ -1385,7 +1421,7 @@
         <v>21</v>
       </c>
       <c r="G49" s="6">
-        <v>800</v>
+        <v>123</v>
       </c>
     </row>
     <row r="50">
@@ -1396,7 +1432,7 @@
         <v>17</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>9</v>
@@ -1405,10 +1441,10 @@
         <v>15</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G50" s="6">
-        <v>300</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="51">
@@ -1419,7 +1455,7 @@
         <v>17</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>9</v>
@@ -1428,10 +1464,10 @@
         <v>15</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G51" s="6">
-        <v>350</v>
+        <v>300</v>
       </c>
     </row>
     <row r="52">
@@ -1439,10 +1475,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>9</v>
@@ -1454,7 +1490,7 @@
         <v>21</v>
       </c>
       <c r="G52" s="6">
-        <v>800</v>
+        <v>9999999999</v>
       </c>
     </row>
     <row r="53">
@@ -1465,7 +1501,7 @@
         <v>17</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>9</v>
@@ -1477,7 +1513,7 @@
         <v>21</v>
       </c>
       <c r="G53" s="6">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="54">
@@ -1485,10 +1521,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>9</v>
@@ -1500,7 +1536,7 @@
         <v>21</v>
       </c>
       <c r="G54" s="6">
-        <v>800</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55">
@@ -1511,7 +1547,7 @@
         <v>17</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>9</v>
@@ -1531,22 +1567,22 @@
         <v>55</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="G56" s="6">
-        <v>560</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="57">
@@ -1554,22 +1590,22 @@
         <v>56</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="G57" s="6">
-        <v>500</v>
+        <v>200</v>
       </c>
     </row>
     <row r="58">
@@ -1580,19 +1616,19 @@
         <v>17</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G58" s="6">
-        <v>400</v>
+        <v>122</v>
       </c>
     </row>
     <row r="59">
@@ -1603,19 +1639,19 @@
         <v>17</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G59" s="6">
-        <v>500</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="60">
@@ -1626,19 +1662,19 @@
         <v>17</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G60" s="6">
-        <v>500</v>
+        <v>800</v>
       </c>
     </row>
     <row r="61">
@@ -1646,22 +1682,22 @@
         <v>60</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="D61" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="G61" s="6">
-        <v>2000</v>
+        <v>99999</v>
       </c>
     </row>
     <row r="62">
@@ -1672,19 +1708,19 @@
         <v>17</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G62" s="6">
-        <v>600</v>
+        <v>300</v>
       </c>
     </row>
     <row r="63">
@@ -1692,22 +1728,22 @@
         <v>62</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G63" s="6">
-        <v>300</v>
+        <v>800</v>
       </c>
     </row>
     <row r="64">
@@ -1715,22 +1751,22 @@
         <v>63</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="G64" s="6">
-        <v>800</v>
+        <v>350</v>
       </c>
     </row>
     <row r="65">
@@ -1738,13 +1774,13 @@
         <v>64</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="E65" s="4" t="s">
         <v>15</v>
@@ -1753,7 +1789,7 @@
         <v>21</v>
       </c>
       <c r="G65" s="6">
-        <v>11</v>
+        <v>800</v>
       </c>
     </row>
     <row r="66">
@@ -1761,22 +1797,22 @@
         <v>65</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="E66" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="G66" s="6">
-        <v>620</v>
+        <v>300</v>
       </c>
     </row>
     <row r="67">
@@ -1784,22 +1820,22 @@
         <v>66</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="E67" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="G67" s="6">
-        <v>820</v>
+        <v>800</v>
       </c>
     </row>
     <row r="68">
@@ -1810,19 +1846,19 @@
         <v>17</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="E68" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="G68" s="6">
-        <v>200</v>
+        <v>800</v>
       </c>
     </row>
     <row r="69">
@@ -1830,22 +1866,22 @@
         <v>68</v>
       </c>
       <c r="B69" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F69" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C69" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E69" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F69" s="4" t="s">
-        <v>45</v>
-      </c>
       <c r="G69" s="6">
-        <v>350</v>
+        <v>560</v>
       </c>
     </row>
     <row r="70">
@@ -1853,19 +1889,19 @@
         <v>69</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C70" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F70" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="D70" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E70" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F70" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="G70" s="6">
         <v>500</v>
@@ -1876,22 +1912,22 @@
         <v>70</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="F71" s="4" t="s">
         <v>16</v>
       </c>
       <c r="G71" s="6">
-        <v>500</v>
+        <v>400</v>
       </c>
     </row>
     <row r="72">
@@ -1899,16 +1935,16 @@
         <v>71</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="F72" s="4" t="s">
         <v>16</v>
@@ -1922,16 +1958,16 @@
         <v>72</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="F73" s="4" t="s">
         <v>16</v>
@@ -1948,19 +1984,19 @@
         <v>12</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="G74" s="6">
-        <v>500</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="75">
@@ -1971,19 +2007,19 @@
         <v>17</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G75" s="6">
-        <v>500</v>
+        <v>600</v>
       </c>
     </row>
     <row r="76">
@@ -1994,19 +2030,19 @@
         <v>17</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G76" s="6">
-        <v>500</v>
+        <v>300</v>
       </c>
     </row>
     <row r="77">
@@ -2014,22 +2050,22 @@
         <v>76</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G77" s="6">
-        <v>500</v>
+        <v>800</v>
       </c>
     </row>
     <row r="78">
@@ -2037,22 +2073,22 @@
         <v>77</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G78" s="6">
-        <v>500</v>
+        <v>11</v>
       </c>
     </row>
     <row r="79">
@@ -2063,19 +2099,19 @@
         <v>12</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="G79" s="6">
-        <v>500</v>
+        <v>620</v>
       </c>
     </row>
     <row r="80">
@@ -2086,19 +2122,19 @@
         <v>12</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="G80" s="6">
-        <v>500</v>
+        <v>820</v>
       </c>
     </row>
     <row r="81">
@@ -2106,22 +2142,22 @@
         <v>80</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="G81" s="6">
-        <v>500</v>
+        <v>200</v>
       </c>
     </row>
     <row r="82">
@@ -2129,22 +2165,22 @@
         <v>81</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="G82" s="6">
-        <v>500</v>
+        <v>350</v>
       </c>
     </row>
     <row r="83">
@@ -2152,22 +2188,22 @@
         <v>82</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G83" s="6">
-        <v>500</v>
+        <v>120</v>
       </c>
     </row>
     <row r="84">
@@ -2175,16 +2211,16 @@
         <v>83</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="F84" s="4" t="s">
         <v>16</v>
@@ -2201,13 +2237,13 @@
         <v>12</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="F85" s="4" t="s">
         <v>16</v>
@@ -2221,16 +2257,16 @@
         <v>85</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="E86" s="4" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="F86" s="4" t="s">
         <v>16</v>
@@ -2244,16 +2280,16 @@
         <v>86</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="F87" s="4" t="s">
         <v>16</v>
@@ -2267,16 +2303,16 @@
         <v>87</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="F88" s="4" t="s">
         <v>16</v>
@@ -2290,16 +2326,16 @@
         <v>88</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="E89" s="4" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="F89" s="4" t="s">
         <v>16</v>
@@ -2313,16 +2349,16 @@
         <v>89</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="E90" s="4" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="F90" s="4" t="s">
         <v>16</v>
@@ -2339,13 +2375,13 @@
         <v>17</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="E91" s="4" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="F91" s="4" t="s">
         <v>16</v>
@@ -2362,19 +2398,19 @@
         <v>17</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="F92" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="G92" s="6">
-        <v>200</v>
+        <v>500</v>
       </c>
     </row>
     <row r="93">
@@ -2382,21 +2418,412 @@
         <v>92</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="C93" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D93" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E93" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F93" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G93" s="6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="5">
+        <v>93</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D94" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E94" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F94" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G94" s="6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="5">
+        <v>94</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E95" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F95" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G95" s="6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="5">
+        <v>95</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E96" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F96" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G96" s="6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="5">
+        <v>96</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E97" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F97" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G97" s="6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="5">
+        <v>97</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C98" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D93" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E93" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F93" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G93" s="6">
+      <c r="D98" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E98" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F98" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G98" s="6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="5">
+        <v>98</v>
+      </c>
+      <c r="B99" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D99" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E99" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F99" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G99" s="6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="5">
+        <v>99</v>
+      </c>
+      <c r="B100" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C100" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D100" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E100" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F100" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G100" s="6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="5">
+        <v>100</v>
+      </c>
+      <c r="B101" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C101" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D101" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E101" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F101" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G101" s="6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="5">
+        <v>101</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C102" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D102" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E102" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F102" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G102" s="6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="5">
+        <v>102</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C103" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D103" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E103" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F103" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G103" s="6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="5">
+        <v>103</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C104" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D104" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E104" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F104" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G104" s="6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="5">
+        <v>104</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C105" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D105" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E105" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F105" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G105" s="6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="5">
+        <v>105</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C106" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D106" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E106" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F106" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G106" s="6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="5">
+        <v>106</v>
+      </c>
+      <c r="B107" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C107" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D107" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E107" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F107" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G107" s="6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="5">
+        <v>107</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C108" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D108" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E108" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F108" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G108" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="5">
+        <v>108</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C109" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D109" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E109" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F109" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G109" s="6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="5">
+        <v>109</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C110" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D110" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E110" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F110" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G110" s="6">
         <v>500</v>
       </c>
     </row>

</xml_diff>